<commit_message>
Upload prediction model input data and last scripts
</commit_message>
<xml_diff>
--- a/Table 1.xlsx
+++ b/Table 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijnzoodsma/Documents/PhD/corona/Postcovid-targeted-proteomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDFAFB8-04B6-0847-9FA7-5C01DF9857AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C956A5-DF6E-D944-B5A0-47AED7C88134}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="-1200" windowWidth="33600" windowHeight="20500" xr2:uid="{8A7D9C4D-8085-814A-8E13-797DA18570DD}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
-  <si>
-    <t>Nr. Of samples</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
   <si>
     <t>Gender (M / F)</t>
   </si>
@@ -139,9 +136,6 @@
   </si>
   <si>
     <t>37 ± 11</t>
-  </si>
-  <si>
-    <t>Table 1: General characteristics</t>
   </si>
   <si>
     <t>Cell counts (* 109 / L)</t>
@@ -336,9 +330,6 @@
     <t>0.01 ± 0.02b</t>
   </si>
   <si>
-    <t>Footnotes: Continuous variables are represented as mean ± standard deviation. a: Information available for 21 / 38 patients. b: Information available for 92 / 113 patients. c: Information available for 156 / 186 patients. d: Information available for 35 / 61 individuals.</t>
-  </si>
-  <si>
     <t>2.1 ± 0.8c</t>
   </si>
   <si>
@@ -361,13 +352,46 @@
   </si>
   <si>
     <t>0.001 ± 0.001d</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Footnotes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Continuous variables are represented as mean ± standard deviation. For the cell count information, superscript denoted values are obtained from (a) 21 / 38 (b) 92 / 113 (c) 156 / 186 (d) 35 / 61 individuals.</t>
+    </r>
+  </si>
+  <si>
+    <t>168 (100%)</t>
+  </si>
+  <si>
+    <t>308 (100%)</t>
+  </si>
+  <si>
+    <t>TO ADD?</t>
+  </si>
+  <si>
+    <t>In footnotes mention Veerdonk et al 2020 and Bonifacius et al 2021?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -400,6 +424,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -469,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -533,17 +565,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -859,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FDD33F-F780-B24C-A566-D62D75C3CCDE}">
-  <dimension ref="A2:K34"/>
+  <dimension ref="A2:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="C31" sqref="C31:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -881,58 +917,55 @@
   <sheetData>
     <row r="2" spans="1:11" s="22" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="22" t="s">
-        <v>38</v>
-      </c>
       <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="24"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="23"/>
+      <c r="J3" s="24"/>
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B5" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -945,81 +978,69 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B6" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="16">
-        <v>168</v>
-      </c>
-      <c r="D6" s="16">
-        <v>308</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="E6" s="16"/>
-      <c r="F6" s="16">
-        <v>38</v>
-      </c>
-      <c r="G6" s="16">
-        <v>113</v>
+      <c r="F6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="H6" s="16"/>
-      <c r="I6" s="16">
-        <v>186</v>
-      </c>
-      <c r="J6" s="16">
-        <v>61</v>
+      <c r="I6" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B7" s="15" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E7" s="16"/>
-      <c r="F7" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="16"/>
+      <c r="F7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="17"/>
       <c r="I7" s="16" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B8" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>19</v>
-      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>4</v>
-      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B9" s="18"/>
+      <c r="B9" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -1030,41 +1051,53 @@
       <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>67</v>
+      </c>
       <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="I10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="15" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
@@ -1072,24 +1105,24 @@
         <v>15</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
@@ -1097,53 +1130,41 @@
         <v>16</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B14" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>13</v>
-      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>13</v>
-      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="16"/>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B15" s="18"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1154,91 +1175,103 @@
       <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B16" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="B16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="F16" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+      <c r="I16" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B17" s="15" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="16" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B18" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="16"/>
       <c r="F18" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B19" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.15">
@@ -1246,154 +1279,140 @@
         <v>23</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B21" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="16" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B22" s="15" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J22" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="26" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B23" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="34" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="C26" s="3"/>
+      <c r="B26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B29" s="23"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B24:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Last update on scripts
</commit_message>
<xml_diff>
--- a/Table 1.xlsx
+++ b/Table 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martijnzoodsma/Documents/PhD/corona/Postcovid-targeted-proteomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C956A5-DF6E-D944-B5A0-47AED7C88134}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB95A95-9CAF-554E-9E73-F52F1D4408B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="-1200" windowWidth="33600" windowHeight="20500" xr2:uid="{8A7D9C4D-8085-814A-8E13-797DA18570DD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8A7D9C4D-8085-814A-8E13-797DA18570DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
   <si>
     <t>Gender (M / F)</t>
   </si>
@@ -33,9 +33,6 @@
     <t>99 / 87</t>
   </si>
   <si>
-    <t>74 / 39</t>
-  </si>
-  <si>
     <t>36 / 25</t>
   </si>
   <si>
@@ -45,18 +42,9 @@
     <t>Plasmablasts</t>
   </si>
   <si>
-    <t>10 / 29</t>
-  </si>
-  <si>
     <t>PCR-proven COVID-19 (n (%))</t>
   </si>
   <si>
-    <t>36 (92%)</t>
-  </si>
-  <si>
-    <t>107 (95%)</t>
-  </si>
-  <si>
     <t>General</t>
   </si>
   <si>
@@ -78,12 +66,6 @@
     <t>Days since symptom offset</t>
   </si>
   <si>
-    <t>117 / 51</t>
-  </si>
-  <si>
-    <t>184 / 124</t>
-  </si>
-  <si>
     <t>Lymphocytes</t>
   </si>
   <si>
@@ -102,9 +84,6 @@
     <t>Monocytes</t>
   </si>
   <si>
-    <t>To add</t>
-  </si>
-  <si>
     <t>67 ± 9</t>
   </si>
   <si>
@@ -142,7 +121,7 @@
   </si>
   <si>
     <r>
-      <t>ICU 
+      <t>Convalescent
 (</t>
     </r>
     <r>
@@ -162,12 +141,119 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> = 168)</t>
+      <t xml:space="preserve"> = 186)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cohort 1: Breda </t>
+  </si>
+  <si>
+    <t>Cohort 2: Nijmegen</t>
+  </si>
+  <si>
+    <t>Cohort 3: Hannover</t>
+  </si>
+  <si>
+    <t>0.6 ± 0.9b</t>
+  </si>
+  <si>
+    <t>0.01 ± 0.04b</t>
+  </si>
+  <si>
+    <t>0.01 ± 0.02b</t>
+  </si>
+  <si>
+    <t>2.1 ± 0.8c</t>
+  </si>
+  <si>
+    <t>1.5 ± 0.6c</t>
+  </si>
+  <si>
+    <t>0.17 ± 0.14c</t>
+  </si>
+  <si>
+    <t>0.002 ± 0.004c</t>
+  </si>
+  <si>
+    <t>1.3 ± 0.4d</t>
+  </si>
+  <si>
+    <t>0.9 ± 0.3d</t>
+  </si>
+  <si>
+    <t>0.14 ± 0.06d</t>
+  </si>
+  <si>
+    <t>0.001 ± 0.001d</t>
+  </si>
+  <si>
+    <t>186 (100%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disease </t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>27 ± 4</t>
+  </si>
+  <si>
+    <t>28 ± 5</t>
+  </si>
+  <si>
+    <r>
+      <t>Healthy 
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">n = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>61)</t>
     </r>
   </si>
   <si>
     <r>
       <t>non-ICU 
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">n = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>106)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ICU 
 (</t>
     </r>
     <r>
@@ -187,8 +273,44 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> = 308)</t>
-    </r>
+      <t xml:space="preserve"> = 37)</t>
+    </r>
+  </si>
+  <si>
+    <t>28 / 9</t>
+  </si>
+  <si>
+    <t>69 / 37</t>
+  </si>
+  <si>
+    <t>34 (92%)</t>
+  </si>
+  <si>
+    <t>100 (93%)</t>
+  </si>
+  <si>
+    <t>5.8 ± 3.5b</t>
+  </si>
+  <si>
+    <t>1.2 ± 2.3b</t>
+  </si>
+  <si>
+    <t>0.8 ± 0.5b</t>
+  </si>
+  <si>
+    <t>0.5 ± 0.5b</t>
+  </si>
+  <si>
+    <t>6.4 ± 3.8b</t>
+  </si>
+  <si>
+    <t>0.005 ± 0.01b</t>
+  </si>
+  <si>
+    <t>0.02 ± 0.02b</t>
+  </si>
+  <si>
+    <t>27 ± 4a</t>
   </si>
   <si>
     <r>
@@ -212,37 +334,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> = 38)</t>
+      <t xml:space="preserve"> = 59)</t>
     </r>
   </si>
   <si>
     <r>
       <t>non-ICU 
-(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>n = 113</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Convalescent
 (</t>
     </r>
     <r>
@@ -262,96 +359,35 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> = 186)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Healthy 
-(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>n = 61</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Cohort 1: Breda </t>
-  </si>
-  <si>
-    <t>Cohort 2: Nijmegen</t>
-  </si>
-  <si>
-    <t>Cohort 3: Hannover</t>
-  </si>
-  <si>
-    <t>0.8 ± 0.5a</t>
-  </si>
-  <si>
-    <t>0.5 ± 0.5a</t>
-  </si>
-  <si>
-    <t>6.6 ± 3.8a</t>
-  </si>
-  <si>
-    <t>0.005 ± 0.01a</t>
-  </si>
-  <si>
-    <t>0.02 ± 0.02a</t>
-  </si>
-  <si>
-    <t>1.0 ± 1.3b</t>
-  </si>
-  <si>
-    <t>0.6 ± 0.9b</t>
-  </si>
-  <si>
-    <t>5.8 ± 3.4b</t>
-  </si>
-  <si>
-    <t>0.01 ± 0.04b</t>
-  </si>
-  <si>
-    <t>0.01 ± 0.02b</t>
-  </si>
-  <si>
-    <t>2.1 ± 0.8c</t>
-  </si>
-  <si>
-    <t>1.5 ± 0.6c</t>
-  </si>
-  <si>
-    <t>0.17 ± 0.14c</t>
-  </si>
-  <si>
-    <t>0.002 ± 0.004c</t>
-  </si>
-  <si>
-    <t>1.3 ± 0.4d</t>
-  </si>
-  <si>
-    <t>0.9 ± 0.3d</t>
-  </si>
-  <si>
-    <t>0.14 ± 0.06d</t>
-  </si>
-  <si>
-    <t>0.001 ± 0.001d</t>
+      <t xml:space="preserve"> = 148)</t>
+    </r>
+  </si>
+  <si>
+    <t>45 / 14</t>
+  </si>
+  <si>
+    <t>88 / 60</t>
+  </si>
+  <si>
+    <t>59 (100%)</t>
+  </si>
+  <si>
+    <t>148 (100%)</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>&lt;2x10-16</t>
+  </si>
+  <si>
+    <t>28 ± 4</t>
+  </si>
+  <si>
+    <t>0.36</t>
   </si>
   <si>
     <r>
@@ -371,20 +407,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>: Continuous variables are represented as mean ± standard deviation. For the cell count information, superscript denoted values are obtained from (a) 21 / 38 (b) 92 / 113 (c) 156 / 186 (d) 35 / 61 individuals.</t>
-    </r>
-  </si>
-  <si>
-    <t>168 (100%)</t>
-  </si>
-  <si>
-    <t>308 (100%)</t>
-  </si>
-  <si>
-    <t>TO ADD?</t>
-  </si>
-  <si>
-    <t>In footnotes mention Veerdonk et al 2020 and Bonifacius et al 2021?</t>
+      <t>: Continuous variables are represented as mean ± standard deviation. For the cell count information, superscript denoted values are obtained from (a) 101 / 105 (b) 106 / 143 (c) 156 / 186 (d) 35 / 61 individuals. Cohort 2 (Nijmegen) was described in Janssen et al (2021). Cohort 3 (Hannover) was partially described in Bonifacius et al (2021). P-values were calculated by anova or chi-square test for continuous variables or categorical variables, respectively.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -501,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -566,20 +590,38 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -895,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FDD33F-F780-B24C-A566-D62D75C3CCDE}">
-  <dimension ref="A2:K33"/>
+  <dimension ref="A2:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:D31"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -910,62 +952,68 @@
     <col min="6" max="7" width="12.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="1.83203125" style="1" customWidth="1"/>
     <col min="9" max="10" width="12.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="2" customWidth="1"/>
-    <col min="12" max="15" width="15.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.6640625" style="1"/>
+    <col min="11" max="11" width="1.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="2" customWidth="1"/>
+    <col min="13" max="16" width="15.83203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" s="22" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="22" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="25"/>
+      <c r="C3" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="34"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="24"/>
+      <c r="F3" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="33"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="33"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="28"/>
+    </row>
+    <row r="4" spans="1:13" s="5" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="10" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="10" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+        <v>51</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B5" s="13" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -975,72 +1023,97 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="K5" s="32"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B6" s="15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+      <c r="K6" s="16"/>
+      <c r="L6" s="31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B7" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="17" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="16" t="s">
         <v>1</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B8" s="18"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+        <v>2</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B8" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>50</v>
+      </c>
       <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B9" s="19" t="s">
-        <v>13</v>
-      </c>
+      <c r="F8" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="16"/>
+      <c r="L8" s="30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B9" s="18"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -1049,121 +1122,129 @@
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>67</v>
-      </c>
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B10" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="16"/>
-      <c r="F10" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>9</v>
-      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B11" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B12" s="15" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B13" s="15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B14" s="15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B14" s="18"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="F14" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B15" s="19" t="s">
-        <v>37</v>
+      <c r="I14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B15" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -1173,246 +1254,276 @@
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B16" s="18"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="16"/>
-      <c r="F16" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>52</v>
-      </c>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B17" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B17" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="16"/>
-      <c r="F17" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>53</v>
-      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
       <c r="H17" s="16"/>
-      <c r="I17" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B18" s="15" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E18" s="16"/>
       <c r="F18" s="16" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.15">
+        <v>42</v>
+      </c>
+      <c r="K18" s="16"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B19" s="15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+      <c r="K19" s="16"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B20" s="15" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B21" s="15" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="16" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B22" s="15" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="J23" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="34" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B29" s="23"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.15">
-      <c r="D33" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="K22" s="16"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B23" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="16"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B24" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="16"/>
+    </row>
+    <row r="25" spans="2:12" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+    </row>
+    <row r="26" spans="2:12" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="31" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="B31" s="23"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B26:L26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>